<commit_message>
feat/Further decoupling of data and visualization.
</commit_message>
<xml_diff>
--- a/threeJS-software-city/data-analyzer/resources/data/Process_models_complexity_metrics.xlsx
+++ b/threeJS-software-city/data-analyzer/resources/data/Process_models_complexity_metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonaslanzlinger/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonaslanzlinger/programming/software-city-project/threeJS-software-city/data-analyzer/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C63060F-A63A-4540-A6BB-52E13AAF10F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C2006-46D6-3B4B-B6CB-05E6CFA3B2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1111,13 +1111,13 @@
   <dimension ref="A1:V116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat/Making visualization of different Data Types work
</commit_message>
<xml_diff>
--- a/threeJS-software-city/data-analyzer/resources/data/Process_models_complexity_metrics.xlsx
+++ b/threeJS-software-city/data-analyzer/resources/data/Process_models_complexity_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonaslanzlinger/programming/software-city-project/threeJS-software-city/data-analyzer/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C2006-46D6-3B4B-B6CB-05E6CFA3B2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD8DD0-DFC5-4F4C-B3EA-B9A895A1E8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:V116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>